<commit_message>
Correction de mini bug
</commit_message>
<xml_diff>
--- a/src/Stolons/wwwroot/bills/Producer/4/2016_18_4.xlsx
+++ b/src/Stolons/wwwroot/bills/Producer/4/2016_18_4.xlsx
@@ -12,12 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Producteur :</t>
-  </si>
-  <si>
-    <t>La ferme de Robert</t>
   </si>
   <si>
     <t>Numéro de facture :</t>
@@ -246,21 +243,19 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>2016</v>
@@ -268,7 +263,7 @@
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>18</v>
@@ -280,10 +275,10 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="C7" s="5">
         <v>4</v>
@@ -291,32 +286,32 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C9" s="13">
         <f>B9*C7</f>
       </c>
       <c r="D9" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="14">
         <f>SUBTOTAL(9,B9)</f>
@@ -327,10 +322,10 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="C12" s="5">
         <v>2</v>
@@ -338,32 +333,32 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="13">
         <f>B14*C12</f>
       </c>
       <c r="D14" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="14">
         <f>SUBTOTAL(9,B14)</f>
@@ -374,10 +369,10 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="5">
         <v>2</v>
@@ -385,32 +380,32 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19" s="13">
         <f>B19*C17</f>
       </c>
       <c r="D19" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="14">
         <f>SUBTOTAL(9,B19)</f>
@@ -421,10 +416,10 @@
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
@@ -432,32 +427,32 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C24" s="13">
         <f>B24*C22</f>
       </c>
       <c r="D24" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B25" s="14">
         <f>SUBTOTAL(9,B24)</f>
@@ -468,10 +463,10 @@
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="5">
         <v>4</v>
@@ -479,32 +474,32 @@
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" s="12">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C29" s="13">
         <f>B29*C27</f>
       </c>
       <c r="D29" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30" s="14">
         <f>SUBTOTAL(9,B29)</f>
@@ -515,7 +510,7 @@
     </row>
     <row r="32">
       <c r="B32" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" s="18">
         <f>C10+C15+C20+C25+C30</f>

</xml_diff>